<commit_message>
working function to fetch excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/CreateBooking.xlsx
+++ b/src/test/resources/CreateBooking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\SelenideRestAssuredCucumberFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7976E087-C0DA-4C80-B6BD-4C295176A590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A95D45F-DEDA-42A2-AB45-D73A9A6CB9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
successfully working fetching data from excel and posting
</commit_message>
<xml_diff>
--- a/src/test/resources/CreateBooking.xlsx
+++ b/src/test/resources/CreateBooking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\SelenideRestAssuredCucumberFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B0BC54-B4E9-478F-8135-29937AEEF033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3F9C9-A77B-44F8-977C-1D9EDB46F7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>firstname</t>
   </si>
@@ -73,13 +73,28 @@
   </si>
   <si>
     <t>Lunch</t>
+  </si>
+  <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
+    <t>2019-01-03</t>
+  </si>
+  <si>
+    <t>2019-01-02</t>
+  </si>
+  <si>
+    <t>2019-01-04</t>
+  </si>
+  <si>
+    <t>2019-01-05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +106,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,10 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,11 +431,12 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:G4"/>
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -449,17 +472,17 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>111</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>43101</v>
-      </c>
-      <c r="F2" s="2">
-        <v>43466</v>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
@@ -472,17 +495,17 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>123</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
-        <v>77612</v>
-      </c>
-      <c r="F3" s="2">
-        <v>77898</v>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
@@ -495,23 +518,24 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>334</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>9987</v>
-      </c>
-      <c r="F4" s="2">
-        <v>79890</v>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>